<commit_message>
update manual book & dataset
</commit_message>
<xml_diff>
--- a/Dataset_HargaEmas_2025.xlsx
+++ b/Dataset_HargaEmas_2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Novandry\Documents\Kuliah\Semester 7\Skripsi\Source Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Novandry\Documents\Kuliah\Semester 7\Skripsi\Source Code\Perancangan Aplikasi  Prediksi Emas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C687C09-DC78-4C92-A55F-748F619F670D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7479FA6-B057-4B42-86B1-E7D89D32699E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5772" yWindow="372" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Harian_Lengkap" sheetId="1" r:id="rId1"/>
@@ -1304,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E298"/>
+  <dimension ref="A1:E305"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="B267" sqref="B267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6385,6 +6385,125 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
+    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A299" s="1">
+        <v>45955</v>
+      </c>
+      <c r="B299">
+        <v>2350000</v>
+      </c>
+      <c r="C299">
+        <v>16728</v>
+      </c>
+      <c r="D299">
+        <v>16561</v>
+      </c>
+      <c r="E299" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A300" s="1">
+        <v>45956</v>
+      </c>
+      <c r="B300">
+        <v>2350000</v>
+      </c>
+      <c r="C300">
+        <v>16728</v>
+      </c>
+      <c r="D300">
+        <v>16561</v>
+      </c>
+      <c r="E300" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A301" s="1">
+        <v>45957</v>
+      </c>
+      <c r="B301">
+        <v>2327000</v>
+      </c>
+      <c r="C301">
+        <v>16713</v>
+      </c>
+      <c r="D301">
+        <v>16546</v>
+      </c>
+      <c r="E301" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A302" s="1">
+        <v>45958</v>
+      </c>
+      <c r="B302">
+        <v>2282000</v>
+      </c>
+      <c r="C302">
+        <v>16711</v>
+      </c>
+      <c r="D302">
+        <v>16544</v>
+      </c>
+      <c r="E302" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A303" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B303">
+        <v>2267000</v>
+      </c>
+      <c r="C303">
+        <v>16705</v>
+      </c>
+      <c r="D303">
+        <v>16538</v>
+      </c>
+      <c r="E303" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A304" s="1">
+        <v>45960</v>
+      </c>
+      <c r="B304">
+        <v>2263000</v>
+      </c>
+      <c r="C304">
+        <v>16714</v>
+      </c>
+      <c r="D304">
+        <v>16547</v>
+      </c>
+      <c r="E304" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A305" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B305">
+        <v>2305000</v>
+      </c>
+      <c r="C305">
+        <v>16723</v>
+      </c>
+      <c r="D305">
+        <v>16556</v>
+      </c>
+      <c r="E305" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
penambahan modul help dan update dataset
</commit_message>
<xml_diff>
--- a/Dataset_HargaEmas_2025.xlsx
+++ b/Dataset_HargaEmas_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Novandry\Documents\Kuliah\Semester 7\Skripsi\Source Code\Perancangan Aplikasi  Prediksi Emas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7479FA6-B057-4B42-86B1-E7D89D32699E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64172A82-EE34-4564-8410-03CD28BA5154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1304,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E305"/>
+  <dimension ref="A1:E313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
-      <selection activeCell="B267" sqref="B267"/>
+    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
+      <selection activeCell="D307" sqref="D307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6504,6 +6504,142 @@
         <v>4.7500000000000001E-2</v>
       </c>
     </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A306" s="1">
+        <v>45962</v>
+      </c>
+      <c r="B306">
+        <v>2290000</v>
+      </c>
+      <c r="C306">
+        <v>16723</v>
+      </c>
+      <c r="D306">
+        <v>16556</v>
+      </c>
+      <c r="E306" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A307" s="1">
+        <v>45963</v>
+      </c>
+      <c r="B307">
+        <v>2290000</v>
+      </c>
+      <c r="C307">
+        <v>16723</v>
+      </c>
+      <c r="D307">
+        <v>16556</v>
+      </c>
+      <c r="E307" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A308" s="1">
+        <v>45964</v>
+      </c>
+      <c r="B308">
+        <v>2278000</v>
+      </c>
+      <c r="C308">
+        <v>16708</v>
+      </c>
+      <c r="D308">
+        <v>16541</v>
+      </c>
+      <c r="E308" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A309" s="1">
+        <v>45965</v>
+      </c>
+      <c r="B309">
+        <v>2286000</v>
+      </c>
+      <c r="C309">
+        <v>16747</v>
+      </c>
+      <c r="D309">
+        <v>16580</v>
+      </c>
+      <c r="E309" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A310" s="1">
+        <v>45966</v>
+      </c>
+      <c r="B310">
+        <v>2260000</v>
+      </c>
+      <c r="C310">
+        <v>16807</v>
+      </c>
+      <c r="D310">
+        <v>16640</v>
+      </c>
+      <c r="E310" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A311" s="1">
+        <v>45967</v>
+      </c>
+      <c r="B311">
+        <v>2287000</v>
+      </c>
+      <c r="C311">
+        <v>16812</v>
+      </c>
+      <c r="D311">
+        <v>16645</v>
+      </c>
+      <c r="E311" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A312" s="1">
+        <v>45968</v>
+      </c>
+      <c r="B312">
+        <v>2296000</v>
+      </c>
+      <c r="C312">
+        <v>16790</v>
+      </c>
+      <c r="D312">
+        <v>16623</v>
+      </c>
+      <c r="E312" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A313" s="1">
+        <v>45969</v>
+      </c>
+      <c r="B313">
+        <v>2299000</v>
+      </c>
+      <c r="C313">
+        <v>16790</v>
+      </c>
+      <c r="D313">
+        <v>16623</v>
+      </c>
+      <c r="E313" s="2">
+        <v>4.7500000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>